<commit_message>
push code of develop
</commit_message>
<xml_diff>
--- a/datas/test_数据整理.xlsx
+++ b/datas/test_数据整理.xlsx
@@ -621,7 +621,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>546</v>
+        <v>557</v>
       </c>
       <c r="G4" t="n">
         <v>43</v>
@@ -813,7 +813,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>398</v>
+        <v>414</v>
       </c>
       <c r="G8" t="n">
         <v>22</v>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G11" t="n">
         <v>25</v>
@@ -1245,7 +1245,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G17" t="n">
         <v>25</v>
@@ -1341,7 +1341,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G19" t="n">
         <v>25</v>
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>912</v>
+        <v>938</v>
       </c>
       <c r="G21" t="n">
         <v>22</v>
@@ -1485,7 +1485,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>5420</v>
+        <v>5421</v>
       </c>
       <c r="G22" t="n">
         <v>205</v>
@@ -1629,7 +1629,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>3427</v>
+        <v>3430</v>
       </c>
       <c r="G25" t="n">
         <v>141</v>
@@ -1869,13 +1869,13 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="G30" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H30" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I30" t="n">
         <v>3</v>
@@ -1917,7 +1917,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="G31" t="n">
         <v>39</v>
@@ -2013,7 +2013,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>1273</v>
+        <v>1279</v>
       </c>
       <c r="G33" t="n">
         <v>84</v>
@@ -2206,7 +2206,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>2019</v>
+        <v>2033</v>
       </c>
       <c r="G37" t="n">
         <v>54</v>
@@ -2350,7 +2350,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>4176</v>
+        <v>4180</v>
       </c>
       <c r="G40" t="n">
         <v>101</v>
@@ -2446,7 +2446,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="G42" t="n">
         <v>47</v>
@@ -2494,7 +2494,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>3213</v>
+        <v>3216</v>
       </c>
       <c r="G43" t="n">
         <v>181</v>
@@ -2639,7 +2639,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="G46" t="n">
         <v>33</v>
@@ -2687,7 +2687,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G47" t="n">
         <v>12</v>
@@ -2735,16 +2735,16 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>17019</v>
+        <v>17130</v>
       </c>
       <c r="G48" t="n">
-        <v>2096</v>
+        <v>2102</v>
       </c>
       <c r="H48" t="n">
-        <v>1128</v>
+        <v>1131</v>
       </c>
       <c r="I48" t="n">
-        <v>923</v>
+        <v>926</v>
       </c>
       <c r="J48" t="n">
         <v>45</v>
@@ -2787,7 +2787,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>4357</v>
+        <v>4358</v>
       </c>
       <c r="G49" t="n">
         <v>528</v>
@@ -2883,16 +2883,16 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>3704</v>
+        <v>3722</v>
       </c>
       <c r="G51" t="n">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H51" t="n">
         <v>167</v>
       </c>
       <c r="I51" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J51" t="n">
         <v>19</v>
@@ -2931,7 +2931,7 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>20916</v>
+        <v>20929</v>
       </c>
       <c r="G52" t="n">
         <v>1258</v>
@@ -2983,7 +2983,7 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>5284</v>
+        <v>5293</v>
       </c>
       <c r="G53" t="n">
         <v>360</v>
@@ -3031,7 +3031,7 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>6299</v>
+        <v>6302</v>
       </c>
       <c r="G54" t="n">
         <v>484</v>
@@ -3079,16 +3079,16 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>31558</v>
+        <v>31781</v>
       </c>
       <c r="G55" t="n">
-        <v>3650</v>
+        <v>3663</v>
       </c>
       <c r="H55" t="n">
-        <v>2268</v>
+        <v>2275</v>
       </c>
       <c r="I55" t="n">
-        <v>1341</v>
+        <v>1347</v>
       </c>
       <c r="J55" t="n">
         <v>41</v>
@@ -3131,7 +3131,7 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>3201</v>
+        <v>3204</v>
       </c>
       <c r="G56" t="n">
         <v>81</v>
@@ -3179,7 +3179,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="G57" t="n">
         <v>40</v>
@@ -3227,7 +3227,7 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>1393</v>
+        <v>1396</v>
       </c>
       <c r="G58" t="n">
         <v>57</v>
@@ -3275,7 +3275,7 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>48339</v>
+        <v>48342</v>
       </c>
       <c r="G59" t="n">
         <v>1779</v>
@@ -3327,7 +3327,7 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>4962</v>
+        <v>4972</v>
       </c>
       <c r="G60" t="n">
         <v>171</v>
@@ -3471,7 +3471,7 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>6882</v>
+        <v>6886</v>
       </c>
       <c r="G63" t="n">
         <v>201</v>
@@ -3569,7 +3569,7 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>1680</v>
+        <v>1686</v>
       </c>
       <c r="G65" t="n">
         <v>54</v>
@@ -3617,7 +3617,7 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="G66" t="n">
         <v>76</v>
@@ -3665,7 +3665,7 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>1430</v>
+        <v>1436</v>
       </c>
       <c r="G67" t="n">
         <v>113</v>
@@ -3761,7 +3761,7 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>3113</v>
+        <v>3116</v>
       </c>
       <c r="G69" t="n">
         <v>90</v>
@@ -3809,7 +3809,7 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>1709</v>
+        <v>1711</v>
       </c>
       <c r="G70" t="n">
         <v>99</v>
@@ -3857,16 +3857,16 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>3483</v>
+        <v>3493</v>
       </c>
       <c r="G71" t="n">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="H71" t="n">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I71" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J71" t="n">
         <v>72</v>
@@ -3953,7 +3953,7 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>7431</v>
+        <v>7433</v>
       </c>
       <c r="G73" t="n">
         <v>320</v>
@@ -4002,7 +4002,7 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>3106</v>
+        <v>3107</v>
       </c>
       <c r="G74" t="n">
         <v>130</v>
@@ -4194,7 +4194,7 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>1140</v>
+        <v>1143</v>
       </c>
       <c r="G78" t="n">
         <v>102</v>
@@ -4242,16 +4242,16 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>33023</v>
+        <v>33356</v>
       </c>
       <c r="G79" t="n">
-        <v>3523</v>
+        <v>3541</v>
       </c>
       <c r="H79" t="n">
-        <v>1987</v>
+        <v>1994</v>
       </c>
       <c r="I79" t="n">
-        <v>1483</v>
+        <v>1494</v>
       </c>
       <c r="J79" t="n">
         <v>53</v>
@@ -4294,13 +4294,13 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>4534</v>
+        <v>4535</v>
       </c>
       <c r="G80" t="n">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H80" t="n">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="I80" t="n">
         <v>36</v>
@@ -4342,16 +4342,16 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>17136</v>
+        <v>17176</v>
       </c>
       <c r="G81" t="n">
         <v>1094</v>
       </c>
       <c r="H81" t="n">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="I81" t="n">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="J81" t="n">
         <v>23</v>
@@ -4394,7 +4394,7 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="G82" t="n">
         <v>78</v>
@@ -4538,7 +4538,7 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>3892</v>
+        <v>3923</v>
       </c>
       <c r="G85" t="n">
         <v>145</v>
@@ -4634,16 +4634,16 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>16808</v>
+        <v>16921</v>
       </c>
       <c r="G87" t="n">
-        <v>1024</v>
+        <v>1028</v>
       </c>
       <c r="H87" t="n">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="I87" t="n">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="J87" t="n">
         <v>122</v>
@@ -4734,7 +4734,7 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>3524</v>
+        <v>3528</v>
       </c>
       <c r="G89" t="n">
         <v>131</v>
@@ -4783,7 +4783,7 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>3742</v>
+        <v>3775</v>
       </c>
       <c r="G90" t="n">
         <v>85</v>
@@ -4834,10 +4834,10 @@
         <v>1564</v>
       </c>
       <c r="G91" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H91" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I91" t="n">
         <v>2</v>
@@ -4927,7 +4927,7 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>2830</v>
+        <v>2888</v>
       </c>
       <c r="G93" t="n">
         <v>40</v>
@@ -4975,7 +4975,7 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>5289</v>
+        <v>5290</v>
       </c>
       <c r="G94" t="n">
         <v>326</v>
@@ -5023,7 +5023,7 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>13950</v>
+        <v>13957</v>
       </c>
       <c r="G95" t="n">
         <v>822</v>
@@ -5071,7 +5071,7 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>6917</v>
+        <v>6932</v>
       </c>
       <c r="G96" t="n">
         <v>218</v>
@@ -5119,7 +5119,7 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>5839</v>
+        <v>5852</v>
       </c>
       <c r="G97" t="n">
         <v>348</v>
@@ -5167,7 +5167,7 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>1903</v>
+        <v>1906</v>
       </c>
       <c r="G98" t="n">
         <v>94</v>
@@ -5215,13 +5215,13 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>9590</v>
+        <v>9640</v>
       </c>
       <c r="G99" t="n">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="H99" t="n">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="I99" t="n">
         <v>178</v>
@@ -5263,7 +5263,7 @@
         </is>
       </c>
       <c r="F100" t="n">
-        <v>1630</v>
+        <v>1632</v>
       </c>
       <c r="G100" t="n">
         <v>69</v>
@@ -5311,7 +5311,7 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>11277</v>
+        <v>11280</v>
       </c>
       <c r="G101" t="n">
         <v>1026</v>
@@ -5363,16 +5363,16 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>3443</v>
+        <v>3445</v>
       </c>
       <c r="G102" t="n">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H102" t="n">
         <v>153</v>
       </c>
       <c r="I102" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J102" t="n">
         <v>105</v>
@@ -5411,7 +5411,7 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>4781</v>
+        <v>4782</v>
       </c>
       <c r="G103" t="n">
         <v>214</v>
@@ -5508,7 +5508,7 @@
         </is>
       </c>
       <c r="F105" t="n">
-        <v>2749</v>
+        <v>2750</v>
       </c>
       <c r="G105" t="n">
         <v>81</v>
@@ -5556,7 +5556,7 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="G106" t="n">
         <v>44</v>
@@ -5604,7 +5604,7 @@
         </is>
       </c>
       <c r="F107" t="n">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="G107" t="n">
         <v>27</v>
@@ -5652,7 +5652,7 @@
         </is>
       </c>
       <c r="F108" t="n">
-        <v>735</v>
+        <v>742</v>
       </c>
       <c r="G108" t="n">
         <v>24</v>
@@ -5700,7 +5700,7 @@
         </is>
       </c>
       <c r="F109" t="n">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="G109" t="n">
         <v>9</v>
@@ -5748,13 +5748,13 @@
         </is>
       </c>
       <c r="F110" t="n">
-        <v>22528</v>
+        <v>22531</v>
       </c>
       <c r="G110" t="n">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="H110" t="n">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="I110" t="n">
         <v>199</v>
@@ -5800,7 +5800,7 @@
         </is>
       </c>
       <c r="F111" t="n">
-        <v>5227</v>
+        <v>5229</v>
       </c>
       <c r="G111" t="n">
         <v>125</v>
@@ -5848,16 +5848,16 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>7293</v>
+        <v>7324</v>
       </c>
       <c r="G112" t="n">
-        <v>1581</v>
+        <v>1583</v>
       </c>
       <c r="H112" t="n">
         <v>808</v>
       </c>
       <c r="I112" t="n">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="J112" t="n">
         <v>18</v>
@@ -5900,16 +5900,16 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>7254</v>
+        <v>7267</v>
       </c>
       <c r="G113" t="n">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H113" t="n">
         <v>270</v>
       </c>
       <c r="I113" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J113" t="n">
         <v>23</v>
@@ -5948,16 +5948,16 @@
         </is>
       </c>
       <c r="F114" t="n">
-        <v>10536</v>
+        <v>10551</v>
       </c>
       <c r="G114" t="n">
-        <v>2148</v>
+        <v>2150</v>
       </c>
       <c r="H114" t="n">
         <v>1123</v>
       </c>
       <c r="I114" t="n">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="J114" t="n">
         <v>13</v>
@@ -6000,16 +6000,16 @@
         </is>
       </c>
       <c r="F115" t="n">
-        <v>10258</v>
+        <v>10393</v>
       </c>
       <c r="G115" t="n">
-        <v>1032</v>
+        <v>1047</v>
       </c>
       <c r="H115" t="n">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="I115" t="n">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="J115" t="n">
         <v>22</v>
@@ -6148,7 +6148,7 @@
         </is>
       </c>
       <c r="F118" t="n">
-        <v>10037</v>
+        <v>10038</v>
       </c>
       <c r="G118" t="n">
         <v>1751</v>
@@ -6296,7 +6296,7 @@
         </is>
       </c>
       <c r="F121" t="n">
-        <v>1175</v>
+        <v>1185</v>
       </c>
       <c r="G121" t="n">
         <v>26</v>
@@ -6344,7 +6344,7 @@
         </is>
       </c>
       <c r="F122" t="n">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="G122" t="n">
         <v>56</v>
@@ -6440,16 +6440,16 @@
         </is>
       </c>
       <c r="F124" t="n">
-        <v>10111</v>
+        <v>10494</v>
       </c>
       <c r="G124" t="n">
-        <v>1715</v>
+        <v>1767</v>
       </c>
       <c r="H124" t="n">
-        <v>1483</v>
+        <v>1529</v>
       </c>
       <c r="I124" t="n">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="J124" t="n">
         <v>35</v>
@@ -6492,13 +6492,13 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>3657</v>
+        <v>3658</v>
       </c>
       <c r="G125" t="n">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H125" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I125" t="n">
         <v>22</v>
@@ -6540,7 +6540,7 @@
         </is>
       </c>
       <c r="F126" t="n">
-        <v>5903</v>
+        <v>5904</v>
       </c>
       <c r="G126" t="n">
         <v>406</v>
@@ -6588,19 +6588,19 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>2088</v>
+        <v>2104</v>
       </c>
       <c r="G127" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H127" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I127" t="n">
         <v>42</v>
       </c>
       <c r="J127" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr">
@@ -6684,7 +6684,7 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>4927</v>
+        <v>4928</v>
       </c>
       <c r="G129" t="n">
         <v>289</v>
@@ -6732,7 +6732,7 @@
         </is>
       </c>
       <c r="F130" t="n">
-        <v>3252</v>
+        <v>3272</v>
       </c>
       <c r="G130" t="n">
         <v>205</v>
@@ -6925,7 +6925,7 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>2761</v>
+        <v>2762</v>
       </c>
       <c r="G134" t="n">
         <v>91</v>
@@ -7069,7 +7069,7 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="G137" t="n">
         <v>23</v>
@@ -7117,13 +7117,13 @@
         </is>
       </c>
       <c r="F138" t="n">
-        <v>14308</v>
+        <v>14320</v>
       </c>
       <c r="G138" t="n">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="H138" t="n">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="I138" t="n">
         <v>202</v>
@@ -7169,7 +7169,7 @@
         </is>
       </c>
       <c r="F139" t="n">
-        <v>9593</v>
+        <v>9598</v>
       </c>
       <c r="G139" t="n">
         <v>387</v>
@@ -7217,7 +7217,7 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>1926</v>
+        <v>1935</v>
       </c>
       <c r="G140" t="n">
         <v>104</v>
@@ -7366,16 +7366,16 @@
         </is>
       </c>
       <c r="F143" t="n">
-        <v>1910</v>
+        <v>1926</v>
       </c>
       <c r="G143" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H143" t="n">
         <v>50</v>
       </c>
       <c r="I143" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J143" t="n">
         <v>3</v>
@@ -7462,7 +7462,7 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>2194</v>
+        <v>2197</v>
       </c>
       <c r="G145" t="n">
         <v>171</v>
@@ -7510,7 +7510,7 @@
         </is>
       </c>
       <c r="F146" t="n">
-        <v>3171</v>
+        <v>3172</v>
       </c>
       <c r="G146" t="n">
         <v>149</v>
@@ -7558,7 +7558,7 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>1906</v>
+        <v>1909</v>
       </c>
       <c r="G147" t="n">
         <v>89</v>
@@ -7702,7 +7702,7 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>4465</v>
+        <v>4472</v>
       </c>
       <c r="G150" t="n">
         <v>256</v>
@@ -7750,16 +7750,16 @@
         </is>
       </c>
       <c r="F151" t="n">
-        <v>22009</v>
+        <v>22321</v>
       </c>
       <c r="G151" t="n">
-        <v>1741</v>
+        <v>1762</v>
       </c>
       <c r="H151" t="n">
-        <v>1117</v>
+        <v>1128</v>
       </c>
       <c r="I151" t="n">
-        <v>543</v>
+        <v>553</v>
       </c>
       <c r="J151" t="n">
         <v>81</v>
@@ -7850,7 +7850,7 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>1940</v>
+        <v>1948</v>
       </c>
       <c r="G153" t="n">
         <v>70</v>
@@ -7898,7 +7898,7 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>4972</v>
+        <v>4976</v>
       </c>
       <c r="G154" t="n">
         <v>283</v>
@@ -7961,7 +7961,7 @@
         </is>
       </c>
       <c r="F156" t="n">
-        <v>16354</v>
+        <v>16369</v>
       </c>
       <c r="G156" t="n">
         <v>922</v>
@@ -8009,7 +8009,7 @@
         </is>
       </c>
       <c r="F157" t="n">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="G157" t="n">
         <v>33</v>
@@ -8057,7 +8057,7 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>2770</v>
+        <v>2774</v>
       </c>
       <c r="G158" t="n">
         <v>66</v>
@@ -8105,13 +8105,13 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>9379</v>
+        <v>9386</v>
       </c>
       <c r="G159" t="n">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="H159" t="n">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I159" t="n">
         <v>98</v>
@@ -8298,7 +8298,7 @@
         </is>
       </c>
       <c r="F163" t="n">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="G163" t="n">
         <v>51</v>
@@ -8346,13 +8346,13 @@
         </is>
       </c>
       <c r="F164" t="n">
-        <v>3255</v>
+        <v>3274</v>
       </c>
       <c r="G164" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H164" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I164" t="n">
         <v>22</v>
@@ -8394,7 +8394,7 @@
         </is>
       </c>
       <c r="F165" t="n">
-        <v>2669</v>
+        <v>2676</v>
       </c>
       <c r="G165" t="n">
         <v>145</v>
@@ -8444,16 +8444,16 @@
         </is>
       </c>
       <c r="F166" t="n">
-        <v>8788</v>
+        <v>8924</v>
       </c>
       <c r="G166" t="n">
-        <v>1208</v>
+        <v>1217</v>
       </c>
       <c r="H166" t="n">
-        <v>650</v>
+        <v>656</v>
       </c>
       <c r="I166" t="n">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="J166" t="n">
         <v>13</v>
@@ -8497,7 +8497,7 @@
         </is>
       </c>
       <c r="F167" t="n">
-        <v>9307</v>
+        <v>9309</v>
       </c>
       <c r="G167" t="n">
         <v>587</v>
@@ -8545,7 +8545,7 @@
         </is>
       </c>
       <c r="F168" t="n">
-        <v>2411</v>
+        <v>2478</v>
       </c>
       <c r="G168" t="n">
         <v>27</v>
@@ -8593,7 +8593,7 @@
         </is>
       </c>
       <c r="F169" t="n">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="G169" t="n">
         <v>57</v>
@@ -8641,7 +8641,7 @@
         </is>
       </c>
       <c r="F170" t="n">
-        <v>2158</v>
+        <v>2181</v>
       </c>
       <c r="G170" t="n">
         <v>102</v>
@@ -8689,16 +8689,16 @@
         </is>
       </c>
       <c r="F171" t="n">
-        <v>38110</v>
+        <v>38116</v>
       </c>
       <c r="G171" t="n">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="H171" t="n">
         <v>2199</v>
       </c>
       <c r="I171" t="n">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="J171" t="n">
         <v>96</v>
@@ -8741,13 +8741,13 @@
         </is>
       </c>
       <c r="F172" t="n">
-        <v>89941</v>
+        <v>89948</v>
       </c>
       <c r="G172" t="n">
-        <v>14988</v>
+        <v>14987</v>
       </c>
       <c r="H172" t="n">
-        <v>13370</v>
+        <v>13369</v>
       </c>
       <c r="I172" t="n">
         <v>1559</v>
@@ -8793,7 +8793,7 @@
         </is>
       </c>
       <c r="F173" t="n">
-        <v>5107</v>
+        <v>5109</v>
       </c>
       <c r="G173" t="n">
         <v>130</v>
@@ -8841,7 +8841,7 @@
         </is>
       </c>
       <c r="F174" t="n">
-        <v>8935</v>
+        <v>8939</v>
       </c>
       <c r="G174" t="n">
         <v>428</v>
@@ -9033,7 +9033,7 @@
         </is>
       </c>
       <c r="F178" t="n">
-        <v>5141</v>
+        <v>5194</v>
       </c>
       <c r="G178" t="n">
         <v>191</v>
@@ -9177,16 +9177,16 @@
         </is>
       </c>
       <c r="F181" t="n">
-        <v>7043</v>
+        <v>7059</v>
       </c>
       <c r="G181" t="n">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H181" t="n">
         <v>346</v>
       </c>
       <c r="I181" t="n">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J181" t="n">
         <v>41</v>
@@ -9225,7 +9225,7 @@
         </is>
       </c>
       <c r="F182" t="n">
-        <v>2952</v>
+        <v>2957</v>
       </c>
       <c r="G182" t="n">
         <v>128</v>
@@ -9275,7 +9275,7 @@
         </is>
       </c>
       <c r="F183" t="n">
-        <v>5440</v>
+        <v>5445</v>
       </c>
       <c r="G183" t="n">
         <v>271</v>
@@ -9371,7 +9371,7 @@
         </is>
       </c>
       <c r="F185" t="n">
-        <v>1154</v>
+        <v>1171</v>
       </c>
       <c r="G185" t="n">
         <v>57</v>
@@ -9419,7 +9419,7 @@
         </is>
       </c>
       <c r="F186" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G186" t="n">
         <v>8</v>
@@ -9467,7 +9467,7 @@
         </is>
       </c>
       <c r="F187" t="n">
-        <v>4751</v>
+        <v>4757</v>
       </c>
       <c r="G187" t="n">
         <v>149</v>
@@ -9515,7 +9515,7 @@
         </is>
       </c>
       <c r="F188" t="n">
-        <v>11508</v>
+        <v>11514</v>
       </c>
       <c r="G188" t="n">
         <v>631</v>
@@ -9611,7 +9611,7 @@
         </is>
       </c>
       <c r="F190" t="n">
-        <v>2645</v>
+        <v>2651</v>
       </c>
       <c r="G190" t="n">
         <v>36</v>
@@ -9659,7 +9659,7 @@
         </is>
       </c>
       <c r="F191" t="n">
-        <v>1622</v>
+        <v>1624</v>
       </c>
       <c r="G191" t="n">
         <v>69</v>
@@ -9707,16 +9707,16 @@
         </is>
       </c>
       <c r="F192" t="n">
-        <v>5015</v>
+        <v>5044</v>
       </c>
       <c r="G192" t="n">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="H192" t="n">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I192" t="n">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J192" t="n">
         <v>19</v>
@@ -9851,7 +9851,7 @@
         </is>
       </c>
       <c r="F195" t="n">
-        <v>1961</v>
+        <v>1962</v>
       </c>
       <c r="G195" t="n">
         <v>76</v>
@@ -9947,7 +9947,7 @@
         </is>
       </c>
       <c r="F197" t="n">
-        <v>1763</v>
+        <v>1764</v>
       </c>
       <c r="G197" t="n">
         <v>88</v>
@@ -9995,7 +9995,7 @@
         </is>
       </c>
       <c r="F198" t="n">
-        <v>2755</v>
+        <v>2775</v>
       </c>
       <c r="G198" t="n">
         <v>105</v>
@@ -10043,7 +10043,7 @@
         </is>
       </c>
       <c r="F199" t="n">
-        <v>1060</v>
+        <v>1064</v>
       </c>
       <c r="G199" t="n">
         <v>73</v>
@@ -10091,7 +10091,7 @@
         </is>
       </c>
       <c r="F200" t="n">
-        <v>4001</v>
+        <v>4011</v>
       </c>
       <c r="G200" t="n">
         <v>212</v>
@@ -10187,16 +10187,16 @@
         </is>
       </c>
       <c r="F202" t="n">
-        <v>1324</v>
+        <v>1326</v>
       </c>
       <c r="G202" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H202" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I202" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J202" t="n">
         <v>4</v>
@@ -10235,7 +10235,7 @@
         </is>
       </c>
       <c r="F203" t="n">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="G203" t="n">
         <v>15</v>
@@ -10331,7 +10331,7 @@
         </is>
       </c>
       <c r="F205" t="n">
-        <v>3537</v>
+        <v>3539</v>
       </c>
       <c r="G205" t="n">
         <v>93</v>
@@ -10475,7 +10475,7 @@
         </is>
       </c>
       <c r="F208" t="n">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="G208" t="n">
         <v>90</v>
@@ -10523,7 +10523,7 @@
         </is>
       </c>
       <c r="F209" t="n">
-        <v>2180</v>
+        <v>2186</v>
       </c>
       <c r="G209" t="n">
         <v>36</v>
@@ -10571,7 +10571,7 @@
         </is>
       </c>
       <c r="F210" t="n">
-        <v>19152</v>
+        <v>19163</v>
       </c>
       <c r="G210" t="n">
         <v>2205</v>
@@ -10623,13 +10623,13 @@
         </is>
       </c>
       <c r="F211" t="n">
-        <v>5377</v>
+        <v>5390</v>
       </c>
       <c r="G211" t="n">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="H211" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I211" t="n">
         <v>130</v>
@@ -10671,7 +10671,7 @@
         </is>
       </c>
       <c r="F212" t="n">
-        <v>3009</v>
+        <v>3013</v>
       </c>
       <c r="G212" t="n">
         <v>161</v>
@@ -10719,13 +10719,13 @@
         </is>
       </c>
       <c r="F213" t="n">
-        <v>30920</v>
+        <v>30960</v>
       </c>
       <c r="G213" t="n">
-        <v>2777</v>
+        <v>2780</v>
       </c>
       <c r="H213" t="n">
-        <v>2470</v>
+        <v>2473</v>
       </c>
       <c r="I213" t="n">
         <v>290</v>
@@ -10869,19 +10869,19 @@
         </is>
       </c>
       <c r="F216" t="n">
-        <v>28560</v>
+        <v>29083</v>
       </c>
       <c r="G216" t="n">
-        <v>5454</v>
+        <v>5526</v>
       </c>
       <c r="H216" t="n">
-        <v>2843</v>
+        <v>2883</v>
       </c>
       <c r="I216" t="n">
-        <v>2524</v>
+        <v>2555</v>
       </c>
       <c r="J216" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K216" t="inlineStr">
         <is>
@@ -11017,13 +11017,13 @@
         </is>
       </c>
       <c r="F219" t="n">
-        <v>3037</v>
+        <v>3133</v>
       </c>
       <c r="G219" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H219" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I219" t="n">
         <v>16</v>
@@ -11115,7 +11115,7 @@
         </is>
       </c>
       <c r="F221" t="n">
-        <v>4063</v>
+        <v>4066</v>
       </c>
       <c r="G221" t="n">
         <v>123</v>
@@ -11163,7 +11163,7 @@
         </is>
       </c>
       <c r="F222" t="n">
-        <v>1821</v>
+        <v>1823</v>
       </c>
       <c r="G222" t="n">
         <v>74</v>
@@ -11211,13 +11211,13 @@
         </is>
       </c>
       <c r="F223" t="n">
-        <v>2981</v>
+        <v>2995</v>
       </c>
       <c r="G223" t="n">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H223" t="n">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I223" t="n">
         <v>70</v>
@@ -11259,7 +11259,7 @@
         </is>
       </c>
       <c r="F224" t="n">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="G224" t="n">
         <v>40</v>
@@ -11355,16 +11355,16 @@
         </is>
       </c>
       <c r="F226" t="n">
-        <v>10108</v>
+        <v>10148</v>
       </c>
       <c r="G226" t="n">
         <v>734</v>
       </c>
       <c r="H226" t="n">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="I226" t="n">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J226" t="n">
         <v>21</v>
@@ -11403,13 +11403,13 @@
         </is>
       </c>
       <c r="F227" t="n">
-        <v>3294</v>
+        <v>3317</v>
       </c>
       <c r="G227" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H227" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I227" t="n">
         <v>45</v>
@@ -11451,7 +11451,7 @@
         </is>
       </c>
       <c r="F228" t="n">
-        <v>11585</v>
+        <v>11592</v>
       </c>
       <c r="G228" t="n">
         <v>651</v>
@@ -11645,7 +11645,7 @@
         </is>
       </c>
       <c r="F232" t="n">
-        <v>713</v>
+        <v>726</v>
       </c>
       <c r="G232" t="n">
         <v>24</v>
@@ -11741,7 +11741,7 @@
         </is>
       </c>
       <c r="F234" t="n">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="G234" t="n">
         <v>21</v>
@@ -11789,7 +11789,7 @@
         </is>
       </c>
       <c r="F235" t="n">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="G235" t="n">
         <v>19</v>
@@ -11837,7 +11837,7 @@
         </is>
       </c>
       <c r="F236" t="n">
-        <v>3255</v>
+        <v>3258</v>
       </c>
       <c r="G236" t="n">
         <v>212</v>
@@ -11935,7 +11935,7 @@
         </is>
       </c>
       <c r="F238" t="n">
-        <v>3890</v>
+        <v>3893</v>
       </c>
       <c r="G238" t="n">
         <v>94</v>
@@ -11983,7 +11983,7 @@
         </is>
       </c>
       <c r="F239" t="n">
-        <v>3127</v>
+        <v>3131</v>
       </c>
       <c r="G239" t="n">
         <v>77</v>
@@ -12031,13 +12031,13 @@
         </is>
       </c>
       <c r="F240" t="n">
-        <v>4737</v>
+        <v>4762</v>
       </c>
       <c r="G240" t="n">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H240" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I240" t="n">
         <v>120</v>
@@ -12079,7 +12079,7 @@
         </is>
       </c>
       <c r="F241" t="n">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="G241" t="n">
         <v>24</v>
@@ -12127,7 +12127,7 @@
         </is>
       </c>
       <c r="F242" t="n">
-        <v>1576</v>
+        <v>1585</v>
       </c>
       <c r="G242" t="n">
         <v>100</v>
@@ -12175,13 +12175,13 @@
         </is>
       </c>
       <c r="F243" t="n">
-        <v>10371</v>
+        <v>10373</v>
       </c>
       <c r="G243" t="n">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="H243" t="n">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="I243" t="n">
         <v>76</v>
@@ -12223,13 +12223,13 @@
         </is>
       </c>
       <c r="F244" t="n">
-        <v>5929</v>
+        <v>5943</v>
       </c>
       <c r="G244" t="n">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H244" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I244" t="n">
         <v>28</v>
@@ -12271,19 +12271,19 @@
         </is>
       </c>
       <c r="F245" t="n">
-        <v>34239</v>
+        <v>34307</v>
       </c>
       <c r="G245" t="n">
-        <v>2863</v>
+        <v>2868</v>
       </c>
       <c r="H245" t="n">
-        <v>2411</v>
+        <v>2413</v>
       </c>
       <c r="I245" t="n">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="J245" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K245" t="inlineStr">
         <is>
@@ -12323,7 +12323,7 @@
         </is>
       </c>
       <c r="F246" t="n">
-        <v>2591</v>
+        <v>2592</v>
       </c>
       <c r="G246" t="n">
         <v>73</v>
@@ -12371,7 +12371,7 @@
         </is>
       </c>
       <c r="F247" t="n">
-        <v>5294</v>
+        <v>5302</v>
       </c>
       <c r="G247" t="n">
         <v>168</v>
@@ -12419,13 +12419,13 @@
         </is>
       </c>
       <c r="F248" t="n">
-        <v>25216</v>
+        <v>25234</v>
       </c>
       <c r="G248" t="n">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H248" t="n">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I248" t="n">
         <v>159</v>
@@ -12467,7 +12467,7 @@
         </is>
       </c>
       <c r="F249" t="n">
-        <v>4996</v>
+        <v>4997</v>
       </c>
       <c r="G249" t="n">
         <v>183</v>
@@ -12563,7 +12563,7 @@
         </is>
       </c>
       <c r="F251" t="n">
-        <v>4270</v>
+        <v>4283</v>
       </c>
       <c r="G251" t="n">
         <v>90</v>
@@ -12611,16 +12611,16 @@
         </is>
       </c>
       <c r="F252" t="n">
-        <v>4183</v>
+        <v>4219</v>
       </c>
       <c r="G252" t="n">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="H252" t="n">
         <v>335</v>
       </c>
       <c r="I252" t="n">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J252" t="n">
         <v>7</v>
@@ -12659,7 +12659,7 @@
         </is>
       </c>
       <c r="F253" t="n">
-        <v>4512</v>
+        <v>4524</v>
       </c>
       <c r="G253" t="n">
         <v>345</v>
@@ -12707,7 +12707,7 @@
         </is>
       </c>
       <c r="F254" t="n">
-        <v>8382</v>
+        <v>8386</v>
       </c>
       <c r="G254" t="n">
         <v>597</v>
@@ -12755,7 +12755,7 @@
         </is>
       </c>
       <c r="F255" t="n">
-        <v>4955</v>
+        <v>4958</v>
       </c>
       <c r="G255" t="n">
         <v>140</v>
@@ -12803,7 +12803,7 @@
         </is>
       </c>
       <c r="F256" t="n">
-        <v>1167</v>
+        <v>1173</v>
       </c>
       <c r="G256" t="n">
         <v>90</v>
@@ -12899,7 +12899,7 @@
         </is>
       </c>
       <c r="F258" t="n">
-        <v>19328</v>
+        <v>19332</v>
       </c>
       <c r="G258" t="n">
         <v>743</v>
@@ -12947,7 +12947,7 @@
         </is>
       </c>
       <c r="F259" t="n">
-        <v>4288</v>
+        <v>4295</v>
       </c>
       <c r="G259" t="n">
         <v>65</v>
@@ -12995,16 +12995,16 @@
         </is>
       </c>
       <c r="F260" t="n">
-        <v>6988</v>
+        <v>7033</v>
       </c>
       <c r="G260" t="n">
-        <v>1807</v>
+        <v>1810</v>
       </c>
       <c r="H260" t="n">
         <v>970</v>
       </c>
       <c r="I260" t="n">
-        <v>821</v>
+        <v>824</v>
       </c>
       <c r="J260" t="n">
         <v>16</v>
@@ -13110,19 +13110,19 @@
         </is>
       </c>
       <c r="F263" t="n">
-        <v>16939</v>
+        <v>16978</v>
       </c>
       <c r="G263" t="n">
-        <v>1238</v>
+        <v>1244</v>
       </c>
       <c r="H263" t="n">
-        <v>925</v>
+        <v>928</v>
       </c>
       <c r="I263" t="n">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="J263" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K263" t="inlineStr">
         <is>
@@ -13177,16 +13177,16 @@
         </is>
       </c>
       <c r="F265" t="n">
-        <v>2140</v>
+        <v>2161</v>
       </c>
       <c r="G265" t="n">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="H265" t="n">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I265" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J265" t="n">
         <v>8</v>
@@ -13225,16 +13225,16 @@
         </is>
       </c>
       <c r="F266" t="n">
-        <v>33930</v>
+        <v>34520</v>
       </c>
       <c r="G266" t="n">
-        <v>3410</v>
+        <v>3461</v>
       </c>
       <c r="H266" t="n">
-        <v>1965</v>
+        <v>1997</v>
       </c>
       <c r="I266" t="n">
-        <v>1412</v>
+        <v>1431</v>
       </c>
       <c r="J266" t="n">
         <v>33</v>
@@ -13277,7 +13277,7 @@
         </is>
       </c>
       <c r="F267" t="n">
-        <v>4536</v>
+        <v>4540</v>
       </c>
       <c r="G267" t="n">
         <v>103</v>
@@ -13325,7 +13325,7 @@
         </is>
       </c>
       <c r="F268" t="n">
-        <v>1685</v>
+        <v>1692</v>
       </c>
       <c r="G268" t="n">
         <v>142</v>
@@ -13421,7 +13421,7 @@
         </is>
       </c>
       <c r="F270" t="n">
-        <v>3949</v>
+        <v>3954</v>
       </c>
       <c r="G270" t="n">
         <v>107</v>
@@ -13469,7 +13469,7 @@
         </is>
       </c>
       <c r="F271" t="n">
-        <v>4844</v>
+        <v>4860</v>
       </c>
       <c r="G271" t="n">
         <v>127</v>
@@ -13517,16 +13517,16 @@
         </is>
       </c>
       <c r="F272" t="n">
-        <v>1356</v>
+        <v>1370</v>
       </c>
       <c r="G272" t="n">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H272" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I272" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J272" t="n">
         <v>6</v>
@@ -13565,7 +13565,7 @@
         </is>
       </c>
       <c r="F273" t="n">
-        <v>3338</v>
+        <v>3375</v>
       </c>
       <c r="G273" t="n">
         <v>205</v>
@@ -13613,13 +13613,13 @@
         </is>
       </c>
       <c r="F274" t="n">
-        <v>6434</v>
+        <v>6445</v>
       </c>
       <c r="G274" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H274" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I274" t="n">
         <v>2</v>
@@ -13661,13 +13661,13 @@
         </is>
       </c>
       <c r="F275" t="n">
-        <v>2551</v>
+        <v>2579</v>
       </c>
       <c r="G275" t="n">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H275" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I275" t="n">
         <v>27</v>
@@ -13767,7 +13767,7 @@
         </is>
       </c>
       <c r="F277" t="n">
-        <v>4831</v>
+        <v>4832</v>
       </c>
       <c r="G277" t="n">
         <v>169</v>
@@ -13815,7 +13815,7 @@
         </is>
       </c>
       <c r="F278" t="n">
-        <v>2849</v>
+        <v>2850</v>
       </c>
       <c r="G278" t="n">
         <v>95</v>
@@ -13911,13 +13911,13 @@
         </is>
       </c>
       <c r="F280" t="n">
-        <v>10064</v>
+        <v>10116</v>
       </c>
       <c r="G280" t="n">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="H280" t="n">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="I280" t="n">
         <v>29</v>
@@ -13959,7 +13959,7 @@
         </is>
       </c>
       <c r="F281" t="n">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="G281" t="n">
         <v>51</v>
@@ -14022,7 +14022,7 @@
         </is>
       </c>
       <c r="F283" t="n">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="G283" t="n">
         <v>18</v>
@@ -14070,7 +14070,7 @@
         </is>
       </c>
       <c r="F284" t="n">
-        <v>2056</v>
+        <v>2062</v>
       </c>
       <c r="G284" t="n">
         <v>102</v>
@@ -14133,7 +14133,7 @@
         </is>
       </c>
       <c r="F286" t="n">
-        <v>1255</v>
+        <v>1257</v>
       </c>
       <c r="G286" t="n">
         <v>85</v>
@@ -14181,7 +14181,7 @@
         </is>
       </c>
       <c r="F287" t="n">
-        <v>1314</v>
+        <v>1319</v>
       </c>
       <c r="G287" t="n">
         <v>68</v>
@@ -14229,16 +14229,16 @@
         </is>
       </c>
       <c r="F288" t="n">
-        <v>14109</v>
+        <v>14242</v>
       </c>
       <c r="G288" t="n">
-        <v>906</v>
+        <v>913</v>
       </c>
       <c r="H288" t="n">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="I288" t="n">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J288" t="n">
         <v>100</v>
@@ -14277,7 +14277,7 @@
         </is>
       </c>
       <c r="F289" t="n">
-        <v>5000</v>
+        <v>5005</v>
       </c>
       <c r="G289" t="n">
         <v>420</v>
@@ -14325,13 +14325,13 @@
         </is>
       </c>
       <c r="F290" t="n">
-        <v>17959</v>
+        <v>17983</v>
       </c>
       <c r="G290" t="n">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="H290" t="n">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="I290" t="n">
         <v>56</v>
@@ -14373,13 +14373,13 @@
         </is>
       </c>
       <c r="F291" t="n">
-        <v>11730</v>
+        <v>11746</v>
       </c>
       <c r="G291" t="n">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="H291" t="n">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="I291" t="n">
         <v>80</v>
@@ -14421,7 +14421,7 @@
         </is>
       </c>
       <c r="F292" t="n">
-        <v>6600</v>
+        <v>6618</v>
       </c>
       <c r="G292" t="n">
         <v>343</v>
@@ -14469,7 +14469,7 @@
         </is>
       </c>
       <c r="F293" t="n">
-        <v>3487</v>
+        <v>3497</v>
       </c>
       <c r="G293" t="n">
         <v>126</v>
@@ -14517,19 +14517,19 @@
         </is>
       </c>
       <c r="F294" t="n">
-        <v>3116</v>
+        <v>3209</v>
       </c>
       <c r="G294" t="n">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="H294" t="n">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="I294" t="n">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J294" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K294" t="inlineStr"/>
       <c r="L294" t="inlineStr">
@@ -14565,7 +14565,7 @@
         </is>
       </c>
       <c r="F295" t="n">
-        <v>3519</v>
+        <v>3523</v>
       </c>
       <c r="G295" t="n">
         <v>98</v>
@@ -14709,16 +14709,16 @@
         </is>
       </c>
       <c r="F298" t="n">
-        <v>19694</v>
+        <v>19735</v>
       </c>
       <c r="G298" t="n">
-        <v>1297</v>
+        <v>1301</v>
       </c>
       <c r="H298" t="n">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="I298" t="n">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="J298" t="n">
         <v>53</v>
@@ -14761,7 +14761,7 @@
         </is>
       </c>
       <c r="F299" t="n">
-        <v>13835</v>
+        <v>13858</v>
       </c>
       <c r="G299" t="n">
         <v>117</v>

</xml_diff>